<commit_message>
Continuing to take behavioral data into multiple columns.
</commit_message>
<xml_diff>
--- a/20170117_CASP_playback_responses_combined_longform.xlsx
+++ b/20170117_CASP_playback_responses_combined_longform.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2487" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>PAIR</t>
+  </si>
+  <si>
+    <t>UNK</t>
   </si>
 </sst>
 </file>
@@ -1136,10 +1139,10 @@
   <dimension ref="A1:V484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="J98" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="K113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L107" sqref="L107"/>
+      <selection pane="bottomRight" activeCell="V125" sqref="V125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -5423,6 +5426,18 @@
       <c r="K109" s="7" t="s">
         <v>74</v>
       </c>
+      <c r="L109" s="1">
+        <v>20</v>
+      </c>
+      <c r="M109" s="1">
+        <v>0</v>
+      </c>
+      <c r="N109" s="1">
+        <v>0</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>230</v>
+      </c>
     </row>
     <row r="110" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
@@ -5455,6 +5470,21 @@
       <c r="K110" s="7" t="s">
         <v>77</v>
       </c>
+      <c r="L110" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N110" s="1">
+        <v>7</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V110" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="111" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
@@ -5487,6 +5517,27 @@
       <c r="K111" s="6" t="s">
         <v>49</v>
       </c>
+      <c r="L111" s="1">
+        <v>30</v>
+      </c>
+      <c r="M111" s="1">
+        <v>300</v>
+      </c>
+      <c r="N111" s="1">
+        <v>4</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>30</v>
+      </c>
+      <c r="R111" s="1">
+        <v>30</v>
+      </c>
+      <c r="S111" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="112" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
@@ -5520,7 +5571,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>41809</v>
       </c>
@@ -5552,7 +5603,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>41809</v>
       </c>
@@ -5584,7 +5635,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>41809</v>
       </c>
@@ -5615,8 +5666,20 @@
       <c r="K115" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L115" s="1">
+        <v>20</v>
+      </c>
+      <c r="M115" s="1">
+        <v>0</v>
+      </c>
+      <c r="N115" s="1">
+        <v>3</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="116" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>41809</v>
       </c>
@@ -5648,7 +5711,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>41809</v>
       </c>
@@ -5680,7 +5743,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>41809</v>
       </c>
@@ -5712,7 +5775,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>41809</v>
       </c>
@@ -5744,7 +5807,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>41809</v>
       </c>
@@ -5776,7 +5839,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>41809</v>
       </c>
@@ -5807,8 +5870,32 @@
       <c r="K121" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L121" s="1">
+        <v>20</v>
+      </c>
+      <c r="M121" s="1">
+        <v>110</v>
+      </c>
+      <c r="N121" s="1">
+        <v>7</v>
+      </c>
+      <c r="O121" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S121" s="1">
+        <v>20</v>
+      </c>
+      <c r="T121" s="1">
+        <v>20</v>
+      </c>
+      <c r="U121" s="1">
+        <v>20</v>
+      </c>
+      <c r="V121" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>41809</v>
       </c>
@@ -5839,8 +5926,23 @@
       <c r="K122" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L122" s="1">
+        <v>30</v>
+      </c>
+      <c r="M122" s="1">
+        <v>0</v>
+      </c>
+      <c r="N122" s="1">
+        <v>2</v>
+      </c>
+      <c r="O122" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q122" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="123" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>41809</v>
       </c>
@@ -5872,7 +5974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>41809</v>
       </c>
@@ -5903,8 +6005,23 @@
       <c r="K124" s="6" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L124" s="1">
+        <v>50</v>
+      </c>
+      <c r="M124" s="1">
+        <v>0</v>
+      </c>
+      <c r="N124" s="1">
+        <v>7</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V124" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>41809</v>
       </c>
@@ -5936,7 +6053,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>41809</v>
       </c>
@@ -5968,7 +6085,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>41809</v>
       </c>
@@ -6000,7 +6117,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>41809</v>
       </c>

</xml_diff>

<commit_message>
More CASP data formatting.
</commit_message>
<xml_diff>
--- a/20170117_CASP_playback_responses_combined_longform.xlsx
+++ b/20170117_CASP_playback_responses_combined_longform.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2487" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -1139,10 +1139,10 @@
   <dimension ref="A1:V484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="K113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="K248" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V125" sqref="V125"/>
+      <selection pane="bottomRight" activeCell="L183" sqref="L183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -6149,7 +6149,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>41809</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>41809</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>41809</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>41809</v>
       </c>
@@ -6276,8 +6276,23 @@
       <c r="K132" s="7" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L132" s="1">
+        <v>30</v>
+      </c>
+      <c r="M132" s="1">
+        <v>180</v>
+      </c>
+      <c r="N132" s="1">
+        <v>2</v>
+      </c>
+      <c r="O132" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q132" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>41809</v>
       </c>
@@ -6309,7 +6324,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>41809</v>
       </c>
@@ -6341,7 +6356,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>41809</v>
       </c>
@@ -6372,8 +6387,20 @@
       <c r="K135" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L135" s="1">
+        <v>20</v>
+      </c>
+      <c r="M135" s="1">
+        <v>265</v>
+      </c>
+      <c r="N135" s="1">
+        <v>2</v>
+      </c>
+      <c r="O135" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>41809</v>
       </c>
@@ -6404,8 +6431,26 @@
       <c r="K136" s="7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L136" s="1">
+        <v>30</v>
+      </c>
+      <c r="M136" s="1">
+        <v>70</v>
+      </c>
+      <c r="N136" s="1">
+        <v>5</v>
+      </c>
+      <c r="O136" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q136" s="1">
+        <v>30</v>
+      </c>
+      <c r="T136" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>41809</v>
       </c>
@@ -6437,7 +6482,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>41809</v>
       </c>
@@ -6468,8 +6513,23 @@
       <c r="K138" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="139" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L138" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N138" s="1">
+        <v>3</v>
+      </c>
+      <c r="O138" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R138" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="139" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>41809</v>
       </c>
@@ -6500,8 +6560,26 @@
       <c r="K139" s="7" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L139" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N139" s="1">
+        <v>5</v>
+      </c>
+      <c r="O139" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R139" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T139" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>41809</v>
       </c>
@@ -6533,7 +6611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>41809</v>
       </c>
@@ -6565,7 +6643,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>41809</v>
       </c>
@@ -6597,7 +6675,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>41788</v>
       </c>
@@ -6631,8 +6709,23 @@
       <c r="K143" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="144" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="L143" s="1">
+        <v>20</v>
+      </c>
+      <c r="M143" s="1">
+        <v>180</v>
+      </c>
+      <c r="N143" s="1">
+        <v>2</v>
+      </c>
+      <c r="O143" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q143" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>41788</v>
       </c>
@@ -6666,8 +6759,26 @@
       <c r="K144" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L144" s="1">
+        <v>20</v>
+      </c>
+      <c r="M144" s="1">
+        <v>90</v>
+      </c>
+      <c r="N144" s="1">
+        <v>7</v>
+      </c>
+      <c r="O144" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q144" s="1">
+        <v>30</v>
+      </c>
+      <c r="V144" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>41788</v>
       </c>
@@ -6702,7 +6813,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="146" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>41788</v>
       </c>
@@ -6736,8 +6847,29 @@
       <c r="K146" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="147" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L146" s="1">
+        <v>30</v>
+      </c>
+      <c r="M146" s="1">
+        <v>90</v>
+      </c>
+      <c r="N146" s="1">
+        <v>7</v>
+      </c>
+      <c r="O146" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q146" s="1">
+        <v>30</v>
+      </c>
+      <c r="R146" s="1">
+        <v>30</v>
+      </c>
+      <c r="V146" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="147" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>41788</v>
       </c>
@@ -6771,8 +6903,26 @@
       <c r="K147" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L147" s="1">
+        <v>20</v>
+      </c>
+      <c r="M147" s="1">
+        <v>10</v>
+      </c>
+      <c r="N147" s="1">
+        <v>6</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q147" s="1">
+        <v>100</v>
+      </c>
+      <c r="U147" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>41788</v>
       </c>
@@ -6806,8 +6956,26 @@
       <c r="K148" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="149" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L148" s="1">
+        <v>40</v>
+      </c>
+      <c r="M148" s="1">
+        <v>300</v>
+      </c>
+      <c r="N148" s="1">
+        <v>7</v>
+      </c>
+      <c r="O148" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q148" s="1">
+        <v>40</v>
+      </c>
+      <c r="V148" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="149" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>41788</v>
       </c>
@@ -6841,8 +7009,29 @@
       <c r="K149" s="6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L149" s="1">
+        <v>20</v>
+      </c>
+      <c r="M149" s="1">
+        <v>180</v>
+      </c>
+      <c r="N149" s="1">
+        <v>7</v>
+      </c>
+      <c r="O149" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q149" s="1">
+        <v>20</v>
+      </c>
+      <c r="U149" s="1">
+        <v>20</v>
+      </c>
+      <c r="V149" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>41788</v>
       </c>
@@ -6876,8 +7065,23 @@
       <c r="K150" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L150" s="1">
+        <v>10</v>
+      </c>
+      <c r="M150" s="1">
+        <v>70</v>
+      </c>
+      <c r="N150" s="1">
+        <v>2</v>
+      </c>
+      <c r="O150" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q150" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>41788</v>
       </c>
@@ -6912,7 +7116,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="152" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>41788</v>
       </c>
@@ -6946,8 +7150,26 @@
       <c r="K152" s="6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="153" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L152" s="1">
+        <v>5</v>
+      </c>
+      <c r="M152" s="1">
+        <v>245</v>
+      </c>
+      <c r="N152" s="1">
+        <v>5</v>
+      </c>
+      <c r="O152" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q152" s="1">
+        <v>30</v>
+      </c>
+      <c r="T152" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>41788</v>
       </c>
@@ -6981,8 +7203,26 @@
       <c r="K153" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="154" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L153" s="1">
+        <v>10</v>
+      </c>
+      <c r="M153" s="1">
+        <v>320</v>
+      </c>
+      <c r="N153" s="1">
+        <v>7</v>
+      </c>
+      <c r="O153" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="R153" s="1">
+        <v>60</v>
+      </c>
+      <c r="V153" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="154" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>41788</v>
       </c>
@@ -7016,8 +7256,29 @@
       <c r="K154" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="155" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L154" s="1">
+        <v>5</v>
+      </c>
+      <c r="M154" s="1">
+        <v>95</v>
+      </c>
+      <c r="N154" s="1">
+        <v>7</v>
+      </c>
+      <c r="O154" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q154" s="1">
+        <v>50</v>
+      </c>
+      <c r="T154" s="1">
+        <v>5</v>
+      </c>
+      <c r="V154" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>41788</v>
       </c>
@@ -7051,8 +7312,26 @@
       <c r="K155" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="156" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L155" s="1">
+        <v>30</v>
+      </c>
+      <c r="M155" s="1">
+        <v>270</v>
+      </c>
+      <c r="N155" s="1">
+        <v>6</v>
+      </c>
+      <c r="O155" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q155" s="1">
+        <v>30</v>
+      </c>
+      <c r="U155" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="156" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>41788</v>
       </c>
@@ -7087,7 +7366,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>41788</v>
       </c>
@@ -7121,8 +7400,20 @@
       <c r="K157" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L157" s="1">
+        <v>20</v>
+      </c>
+      <c r="M157" s="1">
+        <v>0</v>
+      </c>
+      <c r="N157" s="1">
+        <v>2</v>
+      </c>
+      <c r="O157" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="158" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>41788</v>
       </c>
@@ -7156,8 +7447,26 @@
       <c r="K158" s="6" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="159" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L158" s="1">
+        <v>60</v>
+      </c>
+      <c r="M158" s="1">
+        <v>275</v>
+      </c>
+      <c r="N158" s="1">
+        <v>7</v>
+      </c>
+      <c r="O158" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q158" s="1">
+        <v>60</v>
+      </c>
+      <c r="V158" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="159" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>41788</v>
       </c>
@@ -7191,8 +7500,23 @@
       <c r="K159" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="160" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L159" s="1">
+        <v>40</v>
+      </c>
+      <c r="M159" s="1">
+        <v>190</v>
+      </c>
+      <c r="N159" s="1">
+        <v>7</v>
+      </c>
+      <c r="O159" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V159" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="160" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>41788</v>
       </c>
@@ -7226,8 +7550,29 @@
       <c r="K160" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="161" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L160" s="1">
+        <v>10</v>
+      </c>
+      <c r="M160" s="1">
+        <v>180</v>
+      </c>
+      <c r="N160" s="1">
+        <v>7</v>
+      </c>
+      <c r="O160" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q160" s="1">
+        <v>10</v>
+      </c>
+      <c r="S160" s="1">
+        <v>10</v>
+      </c>
+      <c r="V160" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>41788</v>
       </c>
@@ -7261,8 +7606,23 @@
       <c r="K161" s="6" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L161" s="1">
+        <v>30</v>
+      </c>
+      <c r="M161" s="1">
+        <v>190</v>
+      </c>
+      <c r="N161" s="1">
+        <v>2</v>
+      </c>
+      <c r="O161" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q161" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>41788</v>
       </c>
@@ -7297,7 +7657,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:19" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>41788</v>
       </c>
@@ -7331,8 +7691,26 @@
       <c r="K163" s="6" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L163" s="1">
+        <v>20</v>
+      </c>
+      <c r="M163" s="1">
+        <v>265</v>
+      </c>
+      <c r="N163" s="1">
+        <v>3</v>
+      </c>
+      <c r="O163" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q163" s="1">
+        <v>20</v>
+      </c>
+      <c r="R163" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>41788</v>
       </c>
@@ -7367,7 +7745,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:19" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>41788</v>
       </c>
@@ -7401,8 +7779,26 @@
       <c r="K165" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="166" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L165" s="1">
+        <v>40</v>
+      </c>
+      <c r="M165" s="1">
+        <v>90</v>
+      </c>
+      <c r="N165" s="1">
+        <v>4</v>
+      </c>
+      <c r="O165" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q165" s="1">
+        <v>40</v>
+      </c>
+      <c r="S165" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="166" spans="1:19" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>41788</v>
       </c>
@@ -7437,7 +7833,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>41788</v>
       </c>
@@ -7472,7 +7868,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>41813</v>
       </c>
@@ -7504,7 +7900,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>41813</v>
       </c>
@@ -7536,7 +7932,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>41813</v>
       </c>
@@ -7568,7 +7964,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A171" s="3">
         <v>41813</v>
       </c>
@@ -7600,7 +7996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A172" s="3">
         <v>41813</v>
       </c>
@@ -7632,7 +8028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A173" s="3">
         <v>41813</v>
       </c>
@@ -7664,7 +8060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A174" s="3">
         <v>41813</v>
       </c>
@@ -7696,7 +8092,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A175" s="3">
         <v>41813</v>
       </c>
@@ -7727,8 +8123,23 @@
       <c r="K175" s="7" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L175" s="1">
+        <v>50</v>
+      </c>
+      <c r="M175" s="1">
+        <v>90</v>
+      </c>
+      <c r="N175" s="1">
+        <v>4</v>
+      </c>
+      <c r="O175" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S175" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A176" s="3">
         <v>41813</v>
       </c>
@@ -7760,7 +8171,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A177" s="3">
         <v>41813</v>
       </c>
@@ -7792,7 +8203,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A178" s="3">
         <v>41813</v>
       </c>
@@ -7824,7 +8235,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A179" s="3">
         <v>41813</v>
       </c>
@@ -7856,7 +8267,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A180" s="3">
         <v>41813</v>
       </c>
@@ -7888,7 +8299,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="181" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A181" s="3">
         <v>41813</v>
       </c>
@@ -7919,8 +8330,23 @@
       <c r="K181" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="182" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L181" s="1">
+        <v>40</v>
+      </c>
+      <c r="M181" s="1">
+        <v>180</v>
+      </c>
+      <c r="N181" s="1">
+        <v>2</v>
+      </c>
+      <c r="O181" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q181" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="182" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A182" s="3">
         <v>41813</v>
       </c>
@@ -7951,8 +8377,23 @@
       <c r="K182" s="7" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="183" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+      <c r="L182" s="1">
+        <v>100</v>
+      </c>
+      <c r="M182" s="1">
+        <v>180</v>
+      </c>
+      <c r="N182" s="1">
+        <v>7</v>
+      </c>
+      <c r="O182" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V182" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A183" s="3">
         <v>41813</v>
       </c>
@@ -7984,7 +8425,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
         <v>41813</v>
       </c>
@@ -8016,7 +8457,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A185" s="3">
         <v>41813</v>
       </c>
@@ -8048,7 +8489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A186" s="3">
         <v>41813</v>
       </c>
@@ -8080,7 +8521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A187" s="3">
         <v>41813</v>
       </c>
@@ -8112,7 +8553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A188" s="3">
         <v>41813</v>
       </c>
@@ -8144,7 +8585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A189" s="3">
         <v>41813</v>
       </c>
@@ -8176,7 +8617,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="190" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
         <v>41813</v>
       </c>
@@ -8208,7 +8649,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="191" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
         <v>41813</v>
       </c>
@@ -8240,7 +8681,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
         <v>41813</v>
       </c>

</xml_diff>

<commit_message>
Adding sum columns to percent cover to check if adds to 100.  Finished basic expansion of behavior cells for behavior response file.
</commit_message>
<xml_diff>
--- a/20170117_CASP_playback_responses_combined_longform.xlsx
+++ b/20170117_CASP_playback_responses_combined_longform.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2520" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -1139,10 +1139,10 @@
   <dimension ref="A1:V484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="K248" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="K450" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L183" sqref="L183"/>
+      <selection pane="bottomRight" activeCell="L485" sqref="L485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -8424,6 +8424,27 @@
       <c r="K183" s="7" t="s">
         <v>106</v>
       </c>
+      <c r="L183" s="1">
+        <v>10</v>
+      </c>
+      <c r="M183" s="1">
+        <v>0</v>
+      </c>
+      <c r="N183" s="1">
+        <v>6</v>
+      </c>
+      <c r="O183" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q183" s="1">
+        <v>30</v>
+      </c>
+      <c r="S183" s="1">
+        <v>15</v>
+      </c>
+      <c r="U183" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A184" s="3">
@@ -8616,6 +8637,21 @@
       <c r="K189" s="6" t="s">
         <v>107</v>
       </c>
+      <c r="L189" s="1">
+        <v>30</v>
+      </c>
+      <c r="M189" s="1">
+        <v>180</v>
+      </c>
+      <c r="N189" s="1">
+        <v>2</v>
+      </c>
+      <c r="O189" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q189" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="190" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A190" s="3">
@@ -8648,6 +8684,24 @@
       <c r="K190" s="7" t="s">
         <v>108</v>
       </c>
+      <c r="L190" s="1">
+        <v>10</v>
+      </c>
+      <c r="M190" s="1">
+        <v>180</v>
+      </c>
+      <c r="N190" s="1">
+        <v>4</v>
+      </c>
+      <c r="O190" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q190" s="1">
+        <v>10</v>
+      </c>
+      <c r="S190" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="191" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A191" s="3">
@@ -8680,6 +8734,24 @@
       <c r="K191" s="7" t="s">
         <v>109</v>
       </c>
+      <c r="L191" s="1">
+        <v>30</v>
+      </c>
+      <c r="M191" s="1">
+        <v>90</v>
+      </c>
+      <c r="N191" s="1">
+        <v>4</v>
+      </c>
+      <c r="O191" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q191" s="1">
+        <v>30</v>
+      </c>
+      <c r="S191" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A192" s="3">
@@ -8713,7 +8785,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="193" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:21" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A193" s="3">
         <v>41813</v>
       </c>
@@ -8744,8 +8816,26 @@
       <c r="K193" s="6" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L193" s="1">
+        <v>30</v>
+      </c>
+      <c r="M193" s="1">
+        <v>45</v>
+      </c>
+      <c r="N193" s="1">
+        <v>6</v>
+      </c>
+      <c r="O193" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q193" s="1">
+        <v>30</v>
+      </c>
+      <c r="U193" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A194" s="3">
         <v>41813</v>
       </c>
@@ -8776,8 +8866,23 @@
       <c r="K194" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L194" s="1">
+        <v>40</v>
+      </c>
+      <c r="M194" s="1">
+        <v>0</v>
+      </c>
+      <c r="N194" s="1">
+        <v>2</v>
+      </c>
+      <c r="O194" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q194" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A195" s="3">
         <v>41813</v>
       </c>
@@ -8808,8 +8913,23 @@
       <c r="K195" s="6" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L195" s="1">
+        <v>30</v>
+      </c>
+      <c r="M195" s="1">
+        <v>260</v>
+      </c>
+      <c r="N195" s="1">
+        <v>2</v>
+      </c>
+      <c r="O195" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q195" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="196" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A196" s="3">
         <v>41813</v>
       </c>
@@ -8841,7 +8961,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A197" s="3">
         <v>41813</v>
       </c>
@@ -8873,7 +8993,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A198" s="3">
         <v>41813</v>
       </c>
@@ -8905,7 +9025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="199" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:21" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A199" s="3">
         <v>41813</v>
       </c>
@@ -8936,8 +9056,23 @@
       <c r="K199" s="7" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L199" s="1">
+        <v>25</v>
+      </c>
+      <c r="M199" s="1">
+        <v>145</v>
+      </c>
+      <c r="N199" s="1">
+        <v>2</v>
+      </c>
+      <c r="O199" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q199" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="200" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A200" s="3">
         <v>41813</v>
       </c>
@@ -8969,7 +9104,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A201" s="3">
         <v>41813</v>
       </c>
@@ -9001,7 +9136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A202" s="3">
         <v>41813</v>
       </c>
@@ -9033,7 +9168,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A203" s="3">
         <v>41813</v>
       </c>
@@ -9064,8 +9199,23 @@
       <c r="K203" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L203" s="1">
+        <v>20</v>
+      </c>
+      <c r="M203" s="1">
+        <v>270</v>
+      </c>
+      <c r="N203" s="1">
+        <v>2</v>
+      </c>
+      <c r="O203" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q203" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="204" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A204" s="3">
         <v>41813</v>
       </c>
@@ -9097,7 +9247,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A205" s="3">
         <v>41813</v>
       </c>
@@ -9129,7 +9279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A206" s="3">
         <v>41813</v>
       </c>
@@ -9161,7 +9311,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="207" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:21" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A207" s="3">
         <v>41813</v>
       </c>
@@ -9192,8 +9342,23 @@
       <c r="K207" s="7" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L207" s="1">
+        <v>15</v>
+      </c>
+      <c r="M207" s="1">
+        <v>10</v>
+      </c>
+      <c r="N207" s="1">
+        <v>2</v>
+      </c>
+      <c r="O207" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q207" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="208" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A208" s="3">
         <v>41813</v>
       </c>
@@ -9225,7 +9390,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A209" s="3">
         <v>41813</v>
       </c>
@@ -9257,7 +9422,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A210" s="3">
         <v>41813</v>
       </c>
@@ -9289,7 +9454,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A211" s="3">
         <v>41813</v>
       </c>
@@ -9321,7 +9486,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A212" s="3">
         <v>41813</v>
       </c>
@@ -9353,7 +9518,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A213" s="3">
         <v>41813</v>
       </c>
@@ -9385,7 +9550,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A214" s="3">
         <v>41813</v>
       </c>
@@ -9417,7 +9582,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A215" s="3">
         <v>41813</v>
       </c>
@@ -9448,8 +9613,23 @@
       <c r="K215" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L215" s="1">
+        <v>100</v>
+      </c>
+      <c r="M215" s="1">
+        <v>270</v>
+      </c>
+      <c r="N215" s="1">
+        <v>4</v>
+      </c>
+      <c r="O215" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S215" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A216" s="3">
         <v>41813</v>
       </c>
@@ -9481,7 +9661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A217" s="3">
         <v>41813</v>
       </c>
@@ -9513,7 +9693,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A218" s="3">
         <v>41813</v>
       </c>
@@ -9545,7 +9725,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A219" s="3">
         <v>41813</v>
       </c>
@@ -9577,7 +9757,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A220" s="3">
         <v>41813</v>
       </c>
@@ -9609,7 +9789,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A221" s="3">
         <v>41813</v>
       </c>
@@ -9641,7 +9821,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A222" s="3">
         <v>41813</v>
       </c>
@@ -9673,7 +9853,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A223" s="3">
         <v>41813</v>
       </c>
@@ -9704,8 +9884,23 @@
       <c r="K223" s="7" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L223" s="1">
+        <v>100</v>
+      </c>
+      <c r="M223" s="1">
+        <v>270</v>
+      </c>
+      <c r="N223" s="1">
+        <v>4</v>
+      </c>
+      <c r="O223" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S223" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A224" s="3">
         <v>41813</v>
       </c>
@@ -9736,8 +9931,23 @@
       <c r="K224" s="7" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L224" s="1">
+        <v>30</v>
+      </c>
+      <c r="M224" s="1">
+        <v>160</v>
+      </c>
+      <c r="N224" s="1">
+        <v>2</v>
+      </c>
+      <c r="O224" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q224" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="225" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A225" s="3">
         <v>41813</v>
       </c>
@@ -9769,7 +9979,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A226" s="3">
         <v>41813</v>
       </c>
@@ -9801,7 +10011,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A227" s="3">
         <v>41813</v>
       </c>
@@ -9832,8 +10042,26 @@
       <c r="K227" s="7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="228" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L227" s="1">
+        <v>20</v>
+      </c>
+      <c r="M227" s="1">
+        <v>180</v>
+      </c>
+      <c r="N227" s="1">
+        <v>3</v>
+      </c>
+      <c r="O227" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q227" s="1">
+        <v>20</v>
+      </c>
+      <c r="R227" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="228" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A228" s="3">
         <v>41813</v>
       </c>
@@ -9864,8 +10092,23 @@
       <c r="K228" s="7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L228" s="1">
+        <v>20</v>
+      </c>
+      <c r="M228" s="1">
+        <v>0</v>
+      </c>
+      <c r="N228" s="1">
+        <v>4</v>
+      </c>
+      <c r="O228" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S228" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="229" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A229" s="3">
         <v>41813</v>
       </c>
@@ -9897,7 +10140,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A230" s="3">
         <v>41813</v>
       </c>
@@ -9928,8 +10171,32 @@
       <c r="K230" s="7" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="231" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L230" s="1">
+        <v>10</v>
+      </c>
+      <c r="M230" s="1">
+        <v>90</v>
+      </c>
+      <c r="N230" s="1">
+        <v>7</v>
+      </c>
+      <c r="O230" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q230" s="1">
+        <v>10</v>
+      </c>
+      <c r="S230" s="1">
+        <v>40</v>
+      </c>
+      <c r="U230" s="1">
+        <v>10</v>
+      </c>
+      <c r="V230" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A231" s="3">
         <v>41813</v>
       </c>
@@ -9960,8 +10227,26 @@
       <c r="K231" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L231" s="1">
+        <v>10</v>
+      </c>
+      <c r="M231" s="1">
+        <v>0</v>
+      </c>
+      <c r="N231" s="1">
+        <v>5</v>
+      </c>
+      <c r="O231" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S231" s="1">
+        <v>40</v>
+      </c>
+      <c r="T231" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="232" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A232" s="3">
         <v>41821</v>
       </c>
@@ -9993,7 +10278,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A233" s="3">
         <v>41821</v>
       </c>
@@ -10025,7 +10310,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A234" s="3">
         <v>41821</v>
       </c>
@@ -10057,7 +10342,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A235" s="3">
         <v>41821</v>
       </c>
@@ -10089,7 +10374,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A236" s="3">
         <v>41821</v>
       </c>
@@ -10121,7 +10406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A237" s="3">
         <v>41821</v>
       </c>
@@ -10153,7 +10438,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A238" s="3">
         <v>41821</v>
       </c>
@@ -10185,7 +10470,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A239" s="3">
         <v>41821</v>
       </c>
@@ -10217,7 +10502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A240" s="3">
         <v>41821</v>
       </c>
@@ -10249,7 +10534,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A241" s="3">
         <v>41821</v>
       </c>
@@ -10281,7 +10566,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A242" s="3">
         <v>41821</v>
       </c>
@@ -10313,7 +10598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A243" s="3">
         <v>41821</v>
       </c>
@@ -10345,7 +10630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A244" s="3">
         <v>41821</v>
       </c>
@@ -10377,7 +10662,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A245" s="3">
         <v>41821</v>
       </c>
@@ -10409,7 +10694,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A246" s="3">
         <v>41821</v>
       </c>
@@ -10441,7 +10726,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A247" s="3">
         <v>41821</v>
       </c>
@@ -10473,7 +10758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A248" s="3">
         <v>41821</v>
       </c>
@@ -10505,7 +10790,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A249" s="3">
         <v>41821</v>
       </c>
@@ -10537,7 +10822,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A250" s="3">
         <v>41821</v>
       </c>
@@ -10569,7 +10854,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A251" s="3">
         <v>41821</v>
       </c>
@@ -10600,8 +10885,23 @@
       <c r="K251" s="6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L251" s="1">
+        <v>50</v>
+      </c>
+      <c r="M251" s="1">
+        <v>180</v>
+      </c>
+      <c r="N251" s="1">
+        <v>7</v>
+      </c>
+      <c r="O251" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V251" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="252" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A252" s="3">
         <v>41821</v>
       </c>
@@ -10633,7 +10933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A253" s="3">
         <v>41821</v>
       </c>
@@ -10665,7 +10965,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A254" s="3">
         <v>41821</v>
       </c>
@@ -10697,7 +10997,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A255" s="3">
         <v>41821</v>
       </c>
@@ -10729,7 +11029,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A256" s="3">
         <v>41821</v>
       </c>
@@ -10761,7 +11061,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="257" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A257" s="3">
         <v>41821</v>
       </c>
@@ -10792,8 +11092,26 @@
       <c r="K257" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L257" s="1">
+        <v>7</v>
+      </c>
+      <c r="M257" s="1">
+        <v>220</v>
+      </c>
+      <c r="N257" s="1">
+        <v>5</v>
+      </c>
+      <c r="O257" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q257" s="1">
+        <v>7</v>
+      </c>
+      <c r="T257" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A258" s="3">
         <v>41821</v>
       </c>
@@ -10825,7 +11143,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="259" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A259" s="3">
         <v>41821</v>
       </c>
@@ -10856,8 +11174,23 @@
       <c r="K259" s="6" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="260" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L259" s="1">
+        <v>20</v>
+      </c>
+      <c r="M259" s="1">
+        <v>180</v>
+      </c>
+      <c r="N259" s="1">
+        <v>4</v>
+      </c>
+      <c r="O259" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S259" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="260" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A260" s="3">
         <v>41821</v>
       </c>
@@ -10888,8 +11221,26 @@
       <c r="K260" s="6" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="261" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L260" s="1">
+        <v>15</v>
+      </c>
+      <c r="M260" s="1">
+        <v>190</v>
+      </c>
+      <c r="N260" s="1">
+        <v>4</v>
+      </c>
+      <c r="O260" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q260" s="1">
+        <v>15</v>
+      </c>
+      <c r="S260" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="261" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A261" s="3">
         <v>41821</v>
       </c>
@@ -10920,8 +11271,26 @@
       <c r="K261" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L261" s="1">
+        <v>10</v>
+      </c>
+      <c r="M261" s="1">
+        <v>25</v>
+      </c>
+      <c r="N261" s="1">
+        <v>6</v>
+      </c>
+      <c r="O261" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q261" s="1">
+        <v>10</v>
+      </c>
+      <c r="U261" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="262" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A262" s="3">
         <v>41821</v>
       </c>
@@ -10953,7 +11322,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A263" s="3">
         <v>41821</v>
       </c>
@@ -10985,7 +11354,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A264" s="3">
         <v>41821</v>
       </c>
@@ -11016,8 +11385,23 @@
       <c r="K264" s="6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L264" s="1">
+        <v>100</v>
+      </c>
+      <c r="M264" s="1">
+        <v>90</v>
+      </c>
+      <c r="N264" s="1">
+        <v>7</v>
+      </c>
+      <c r="O264" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V264" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="265" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A265" s="3">
         <v>41821</v>
       </c>
@@ -11049,7 +11433,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A266" s="3">
         <v>41821</v>
       </c>
@@ -11081,7 +11465,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A267" s="3">
         <v>41821</v>
       </c>
@@ -11112,8 +11496,23 @@
       <c r="K267" s="6" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L267" s="1">
+        <v>20</v>
+      </c>
+      <c r="M267" s="1">
+        <v>90</v>
+      </c>
+      <c r="N267" s="1">
+        <v>2</v>
+      </c>
+      <c r="O267" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q267" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="268" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A268" s="3">
         <v>41821</v>
       </c>
@@ -11145,7 +11544,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A269" s="3">
         <v>41821</v>
       </c>
@@ -11177,7 +11576,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A270" s="3">
         <v>41821</v>
       </c>
@@ -11209,7 +11608,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A271" s="3">
         <v>41821</v>
       </c>
@@ -11241,7 +11640,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="272" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A272" s="3">
         <v>41821</v>
       </c>
@@ -11272,8 +11671,23 @@
       <c r="K272" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L272" s="1">
+        <v>50</v>
+      </c>
+      <c r="M272" s="1">
+        <v>0</v>
+      </c>
+      <c r="N272" s="1">
+        <v>3</v>
+      </c>
+      <c r="O272" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R272" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="273" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A273" s="3">
         <v>41821</v>
       </c>
@@ -11305,7 +11719,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A274" s="3">
         <v>41821</v>
       </c>
@@ -11337,7 +11751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A275" s="3">
         <v>41821</v>
       </c>
@@ -11369,7 +11783,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A276" s="3">
         <v>41821</v>
       </c>
@@ -11401,7 +11815,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A277" s="3">
         <v>41821</v>
       </c>
@@ -11433,7 +11847,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A278" s="3">
         <v>41821</v>
       </c>
@@ -11465,7 +11879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A279" s="3">
         <v>41821</v>
       </c>
@@ -11497,7 +11911,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="280" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A280" s="3">
         <v>41821</v>
       </c>
@@ -11528,8 +11942,26 @@
       <c r="K280" s="7" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L280" s="1">
+        <v>10</v>
+      </c>
+      <c r="M280" s="1">
+        <v>25</v>
+      </c>
+      <c r="N280" s="1">
+        <v>7</v>
+      </c>
+      <c r="O280" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="U280" s="1">
+        <v>30</v>
+      </c>
+      <c r="V280" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A281" s="3">
         <v>41821</v>
       </c>
@@ -11561,7 +11993,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A282" s="3">
         <v>41821</v>
       </c>
@@ -11593,7 +12025,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A283" s="3">
         <v>41821</v>
       </c>
@@ -11625,7 +12057,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A284" s="3">
         <v>41821</v>
       </c>
@@ -11657,7 +12089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A285" s="3">
         <v>41821</v>
       </c>
@@ -11689,7 +12121,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A286" s="3">
         <v>41821</v>
       </c>
@@ -11721,7 +12153,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A287" s="3">
         <v>41821</v>
       </c>
@@ -11753,7 +12185,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A288" s="3">
         <v>41821</v>
       </c>
@@ -11785,7 +12217,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A289" s="3">
         <v>41821</v>
       </c>
@@ -11817,7 +12249,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A290" s="3">
         <v>41821</v>
       </c>
@@ -11849,7 +12281,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A291" s="3">
         <v>41821</v>
       </c>
@@ -11881,7 +12313,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A292" s="3">
         <v>41821</v>
       </c>
@@ -11913,7 +12345,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A293" s="3">
         <v>41821</v>
       </c>
@@ -11945,7 +12377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A294" s="3">
         <v>41821</v>
       </c>
@@ -11977,7 +12409,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A295" s="3">
         <v>41821</v>
       </c>
@@ -12009,7 +12441,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A296" s="3">
         <v>41808</v>
       </c>
@@ -12038,7 +12470,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="297" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A297" s="3">
         <v>41808</v>
       </c>
@@ -12069,8 +12501,23 @@
       <c r="K297" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="298" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L297" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M297" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N297" s="1">
+        <v>6</v>
+      </c>
+      <c r="O297" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="U297" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="298" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A298" s="3">
         <v>41808</v>
       </c>
@@ -12101,8 +12548,32 @@
       <c r="K298" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L298" s="1">
+        <v>20</v>
+      </c>
+      <c r="M298" s="1">
+        <v>180</v>
+      </c>
+      <c r="N298" s="1">
+        <v>7</v>
+      </c>
+      <c r="O298" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q298" s="1">
+        <v>20</v>
+      </c>
+      <c r="R298" s="1">
+        <v>20</v>
+      </c>
+      <c r="U298" s="1">
+        <v>20</v>
+      </c>
+      <c r="V298" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="299" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A299" s="3">
         <v>41808</v>
       </c>
@@ -12134,7 +12605,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="300" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A300" s="3">
         <v>41808</v>
       </c>
@@ -12165,8 +12636,23 @@
       <c r="K300" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L300" s="1">
+        <v>20</v>
+      </c>
+      <c r="M300" s="1">
+        <v>270</v>
+      </c>
+      <c r="N300" s="1">
+        <v>4</v>
+      </c>
+      <c r="O300" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S300" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="301" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A301" s="3">
         <v>41808</v>
       </c>
@@ -12198,7 +12684,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A302" s="3">
         <v>41808</v>
       </c>
@@ -12230,7 +12716,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="303" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A303" s="3">
         <v>41808</v>
       </c>
@@ -12261,8 +12747,23 @@
       <c r="K303" s="7" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L303" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M303" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N303" s="1">
+        <v>2</v>
+      </c>
+      <c r="O303" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q303" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="304" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A304" s="3">
         <v>41808</v>
       </c>
@@ -12294,7 +12795,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="305" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A305" s="3">
         <v>41808</v>
       </c>
@@ -12325,8 +12826,29 @@
       <c r="K305" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L305" s="1">
+        <v>40</v>
+      </c>
+      <c r="M305" s="1">
+        <v>325</v>
+      </c>
+      <c r="N305" s="1">
+        <v>7</v>
+      </c>
+      <c r="O305" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R305" s="1">
+        <v>40</v>
+      </c>
+      <c r="S305" s="1">
+        <v>40</v>
+      </c>
+      <c r="V305" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="306" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A306" s="3">
         <v>41808</v>
       </c>
@@ -12357,8 +12879,23 @@
       <c r="K306" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L306" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M306" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N306" s="1">
+        <v>7</v>
+      </c>
+      <c r="O306" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V306" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="307" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A307" s="3">
         <v>41808</v>
       </c>
@@ -12390,7 +12927,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="308" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A308" s="3">
         <v>41808</v>
       </c>
@@ -12421,8 +12958,26 @@
       <c r="K308" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L308" s="1">
+        <v>30</v>
+      </c>
+      <c r="M308" s="1">
+        <v>80</v>
+      </c>
+      <c r="N308" s="1">
+        <v>3</v>
+      </c>
+      <c r="O308" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q308" s="1">
+        <v>30</v>
+      </c>
+      <c r="R308" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="309" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A309" s="3">
         <v>41808</v>
       </c>
@@ -12454,7 +13009,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="310" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A310" s="3">
         <v>41808</v>
       </c>
@@ -12486,7 +13041,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="311" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A311" s="3">
         <v>41808</v>
       </c>
@@ -12517,8 +13072,29 @@
       <c r="K311" s="7" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L311" s="1">
+        <v>20</v>
+      </c>
+      <c r="M311" s="1">
+        <v>270</v>
+      </c>
+      <c r="N311" s="1">
+        <v>7</v>
+      </c>
+      <c r="O311" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q311" s="1">
+        <v>20</v>
+      </c>
+      <c r="U311" s="1">
+        <v>20</v>
+      </c>
+      <c r="V311" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="312" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A312" s="3">
         <v>41808</v>
       </c>
@@ -12550,7 +13126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A313" s="3">
         <v>41808</v>
       </c>
@@ -12582,7 +13158,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A314" s="3">
         <v>41808</v>
       </c>
@@ -12613,8 +13189,23 @@
       <c r="K314" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="315" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L314" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M314" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N314" s="1">
+        <v>3</v>
+      </c>
+      <c r="O314" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R314" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="315" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A315" s="3">
         <v>41808</v>
       </c>
@@ -12645,8 +13236,26 @@
       <c r="K315" s="6" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="316" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L315" s="1">
+        <v>50</v>
+      </c>
+      <c r="M315" s="1">
+        <v>60</v>
+      </c>
+      <c r="N315" s="1">
+        <v>5</v>
+      </c>
+      <c r="O315" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q315" s="1">
+        <v>50</v>
+      </c>
+      <c r="T315" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="316" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A316" s="3">
         <v>41808</v>
       </c>
@@ -12677,8 +13286,23 @@
       <c r="K316" s="6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L316" s="1">
+        <v>15</v>
+      </c>
+      <c r="M316" s="1">
+        <v>90</v>
+      </c>
+      <c r="N316" s="1">
+        <v>2</v>
+      </c>
+      <c r="O316" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q316" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="317" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A317" s="3">
         <v>41808</v>
       </c>
@@ -12710,7 +13334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A318" s="3">
         <v>41808</v>
       </c>
@@ -12741,8 +13365,23 @@
       <c r="K318" s="7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L318" s="1">
+        <v>30</v>
+      </c>
+      <c r="M318" s="1">
+        <v>45</v>
+      </c>
+      <c r="N318" s="1">
+        <v>2</v>
+      </c>
+      <c r="O318" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q318" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="319" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A319" s="3">
         <v>41808</v>
       </c>
@@ -12774,7 +13413,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A320" s="3">
         <v>41808</v>
       </c>
@@ -12806,7 +13445,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A321" s="3">
         <v>41808</v>
       </c>
@@ -12837,8 +13476,29 @@
       <c r="K321" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L321" s="1">
+        <v>20</v>
+      </c>
+      <c r="M321" s="1">
+        <v>245</v>
+      </c>
+      <c r="N321" s="1">
+        <v>7</v>
+      </c>
+      <c r="O321" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q321" s="1">
+        <v>20</v>
+      </c>
+      <c r="T321" s="1">
+        <v>20</v>
+      </c>
+      <c r="V321" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="322" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A322" s="3">
         <v>41808</v>
       </c>
@@ -12870,7 +13530,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A323" s="3">
         <v>41808</v>
       </c>
@@ -12901,8 +13561,26 @@
       <c r="K323" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="324" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L323" s="1">
+        <v>5</v>
+      </c>
+      <c r="M323" s="1">
+        <v>180</v>
+      </c>
+      <c r="N323" s="1">
+        <v>6</v>
+      </c>
+      <c r="O323" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q323" s="1">
+        <v>5</v>
+      </c>
+      <c r="U323" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="324" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A324" s="3">
         <v>41808</v>
       </c>
@@ -12933,8 +13611,26 @@
       <c r="K324" s="6" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="325" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L324" s="1">
+        <v>20</v>
+      </c>
+      <c r="M324" s="1">
+        <v>270</v>
+      </c>
+      <c r="N324" s="1">
+        <v>7</v>
+      </c>
+      <c r="O324" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q324" s="1">
+        <v>20</v>
+      </c>
+      <c r="V324" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="325" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A325" s="3">
         <v>41808</v>
       </c>
@@ -12965,8 +13661,23 @@
       <c r="K325" s="6" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L325" s="1">
+        <v>100</v>
+      </c>
+      <c r="M325" s="1">
+        <v>90</v>
+      </c>
+      <c r="N325" s="1">
+        <v>2</v>
+      </c>
+      <c r="O325" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q325" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="326" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A326" s="3">
         <v>41808</v>
       </c>
@@ -12998,7 +13709,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A327" s="3">
         <v>41808</v>
       </c>
@@ -13030,7 +13741,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A328" s="3">
         <v>41808</v>
       </c>
@@ -13062,7 +13773,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A329" s="3">
         <v>41808</v>
       </c>
@@ -13094,7 +13805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A330" s="3">
         <v>41808</v>
       </c>
@@ -13126,7 +13837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A331" s="3">
         <v>41808</v>
       </c>
@@ -13158,7 +13869,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="332" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A332" s="3">
         <v>41808</v>
       </c>
@@ -13189,8 +13900,26 @@
       <c r="K332" s="6" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="333" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L332" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M332" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N332" s="1">
+        <v>7</v>
+      </c>
+      <c r="O332" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q332" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V332" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="333" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A333" s="3">
         <v>41808</v>
       </c>
@@ -13221,8 +13950,26 @@
       <c r="K333" s="6" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L333" s="1">
+        <v>15</v>
+      </c>
+      <c r="M333" s="1">
+        <v>90</v>
+      </c>
+      <c r="N333" s="1">
+        <v>5</v>
+      </c>
+      <c r="O333" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q333" s="1">
+        <v>15</v>
+      </c>
+      <c r="T333" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="334" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A334" s="3">
         <v>41808</v>
       </c>
@@ -13254,7 +14001,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A335" s="3">
         <v>41808</v>
       </c>
@@ -13286,7 +14033,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A336" s="3">
         <v>41808</v>
       </c>
@@ -13318,7 +14065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A337" s="3">
         <v>41808</v>
       </c>
@@ -13350,7 +14097,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A338" s="3">
         <v>41808</v>
       </c>
@@ -13382,7 +14129,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="339" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A339" s="3">
         <v>41808</v>
       </c>
@@ -13413,8 +14160,29 @@
       <c r="K339" s="6" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L339" s="1">
+        <v>100</v>
+      </c>
+      <c r="M339" s="1">
+        <v>90</v>
+      </c>
+      <c r="N339" s="1">
+        <v>7</v>
+      </c>
+      <c r="O339" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q339" s="1">
+        <v>100</v>
+      </c>
+      <c r="R339" s="1">
+        <v>100</v>
+      </c>
+      <c r="V339" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="340" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A340" s="3">
         <v>41808</v>
       </c>
@@ -13445,8 +14213,23 @@
       <c r="K340" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L340" s="1">
+        <v>10</v>
+      </c>
+      <c r="M340" s="1">
+        <v>0</v>
+      </c>
+      <c r="N340" s="1">
+        <v>2</v>
+      </c>
+      <c r="O340" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q340" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="341" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A341" s="3">
         <v>41808</v>
       </c>
@@ -13477,8 +14260,23 @@
       <c r="K341" s="6" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L341" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M341" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N341" s="1">
+        <v>2</v>
+      </c>
+      <c r="O341" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q341" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="342" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A342" s="3">
         <v>41808</v>
       </c>
@@ -13509,8 +14307,23 @@
       <c r="K342" s="7" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L342" s="1">
+        <v>30</v>
+      </c>
+      <c r="M342" s="1">
+        <v>270</v>
+      </c>
+      <c r="N342" s="1">
+        <v>2</v>
+      </c>
+      <c r="O342" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q342" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="343" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A343" s="3">
         <v>41808</v>
       </c>
@@ -13542,7 +14355,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A344" s="3">
         <v>41808</v>
       </c>
@@ -13574,7 +14387,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A345" s="3">
         <v>41808</v>
       </c>
@@ -13606,7 +14419,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A346" s="3">
         <v>41808</v>
       </c>
@@ -13638,7 +14451,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="347" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A347" s="3">
         <v>41808</v>
       </c>
@@ -13669,8 +14482,26 @@
       <c r="K347" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L347" s="1">
+        <v>40</v>
+      </c>
+      <c r="M347" s="1">
+        <v>0</v>
+      </c>
+      <c r="N347" s="1">
+        <v>5</v>
+      </c>
+      <c r="O347" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q347" s="1">
+        <v>100</v>
+      </c>
+      <c r="T347" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="348" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A348" s="3">
         <v>41808</v>
       </c>
@@ -13701,8 +14532,23 @@
       <c r="K348" s="7" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="349" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L348" s="1">
+        <v>100</v>
+      </c>
+      <c r="M348" s="1">
+        <v>190</v>
+      </c>
+      <c r="N348" s="1">
+        <v>2</v>
+      </c>
+      <c r="O348" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q348" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="349" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A349" s="3">
         <v>41808</v>
       </c>
@@ -13733,8 +14579,23 @@
       <c r="K349" s="7" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L349" s="1">
+        <v>20</v>
+      </c>
+      <c r="M349" s="1">
+        <v>345</v>
+      </c>
+      <c r="N349" s="1">
+        <v>2</v>
+      </c>
+      <c r="O349" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q349" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="350" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A350" s="3">
         <v>41808</v>
       </c>
@@ -13766,7 +14627,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A351" s="3">
         <v>41808</v>
       </c>
@@ -13798,7 +14659,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A352" s="3">
         <v>41808</v>
       </c>
@@ -13830,7 +14691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A353" s="3">
         <v>41808</v>
       </c>
@@ -13862,7 +14723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="354" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A354" s="3">
         <v>41808</v>
       </c>
@@ -13893,8 +14754,26 @@
       <c r="K354" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="355" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L354" s="1">
+        <v>20</v>
+      </c>
+      <c r="M354" s="1">
+        <v>10</v>
+      </c>
+      <c r="N354" s="1">
+        <v>6</v>
+      </c>
+      <c r="O354" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q354" s="1">
+        <v>20</v>
+      </c>
+      <c r="U354" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="355" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A355" s="3">
         <v>41808</v>
       </c>
@@ -13925,8 +14804,29 @@
       <c r="K355" s="7" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L355" s="1">
+        <v>30</v>
+      </c>
+      <c r="M355" s="1">
+        <v>90</v>
+      </c>
+      <c r="N355" s="1">
+        <v>7</v>
+      </c>
+      <c r="O355" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q355" s="1">
+        <v>30</v>
+      </c>
+      <c r="S355" s="1">
+        <v>30</v>
+      </c>
+      <c r="V355" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="356" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A356" s="3">
         <v>41808</v>
       </c>
@@ -13958,7 +14858,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A357" s="3">
         <v>41808</v>
       </c>
@@ -13990,7 +14890,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A358" s="3">
         <v>41808</v>
       </c>
@@ -14022,7 +14922,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A359" s="3">
         <v>41808</v>
       </c>
@@ -14054,7 +14954,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="360" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A360" s="3">
         <v>41789</v>
       </c>
@@ -14088,8 +14988,29 @@
       <c r="K360" s="6" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="361" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+      <c r="L360" s="1">
+        <v>30</v>
+      </c>
+      <c r="M360" s="1">
+        <v>185</v>
+      </c>
+      <c r="N360" s="1">
+        <v>7</v>
+      </c>
+      <c r="O360" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q360" s="1">
+        <v>30</v>
+      </c>
+      <c r="U360" s="1">
+        <v>30</v>
+      </c>
+      <c r="V360" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="361" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A361" s="3">
         <v>41789</v>
       </c>
@@ -14123,8 +15044,32 @@
       <c r="K361" s="6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L361" s="1">
+        <v>30</v>
+      </c>
+      <c r="M361" s="1">
+        <v>0</v>
+      </c>
+      <c r="N361" s="1">
+        <v>7</v>
+      </c>
+      <c r="O361" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q361" s="1">
+        <v>30</v>
+      </c>
+      <c r="R361" s="1">
+        <v>60</v>
+      </c>
+      <c r="T361" s="1">
+        <v>30</v>
+      </c>
+      <c r="V361" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="362" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A362" s="3">
         <v>41789</v>
       </c>
@@ -14159,7 +15104,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A363" s="3">
         <v>41789</v>
       </c>
@@ -14193,8 +15138,26 @@
       <c r="K363" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L363" s="1">
+        <v>30</v>
+      </c>
+      <c r="M363" s="1">
+        <v>90</v>
+      </c>
+      <c r="N363" s="1">
+        <v>5</v>
+      </c>
+      <c r="O363" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q363" s="1">
+        <v>30</v>
+      </c>
+      <c r="T363" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="364" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A364" s="3">
         <v>41789</v>
       </c>
@@ -14229,7 +15192,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="365" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A365" s="3">
         <v>41789</v>
       </c>
@@ -14263,8 +15226,29 @@
       <c r="K365" s="6" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="366" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L365" s="1">
+        <v>20</v>
+      </c>
+      <c r="M365" s="1">
+        <v>90</v>
+      </c>
+      <c r="N365" s="1">
+        <v>5</v>
+      </c>
+      <c r="O365" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q365" s="1">
+        <v>20</v>
+      </c>
+      <c r="R365" s="1">
+        <v>40</v>
+      </c>
+      <c r="T365" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="366" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A366" s="3">
         <v>41789</v>
       </c>
@@ -14298,8 +15282,29 @@
       <c r="K366" s="6" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L366" s="1">
+        <v>15</v>
+      </c>
+      <c r="M366" s="1">
+        <v>45</v>
+      </c>
+      <c r="N366" s="1">
+        <v>7</v>
+      </c>
+      <c r="O366" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q366" s="1">
+        <v>30</v>
+      </c>
+      <c r="U366" s="1">
+        <v>15</v>
+      </c>
+      <c r="V366" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="367" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A367" s="3">
         <v>41789</v>
       </c>
@@ -14333,8 +15338,23 @@
       <c r="K367" s="6" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="368" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L367" s="1">
+        <v>80</v>
+      </c>
+      <c r="M367" s="1">
+        <v>0</v>
+      </c>
+      <c r="N367" s="1">
+        <v>2</v>
+      </c>
+      <c r="O367" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q367" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="368" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A368" s="3">
         <v>41789</v>
       </c>
@@ -14368,8 +15388,23 @@
       <c r="K368" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L368" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M368" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N368" s="1">
+        <v>1</v>
+      </c>
+      <c r="O368" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="P368" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="369" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A369" s="3">
         <v>41789</v>
       </c>
@@ -14404,7 +15439,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A370" s="3">
         <v>41789</v>
       </c>
@@ -14439,7 +15474,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A371" s="3">
         <v>41789</v>
       </c>
@@ -14473,8 +15508,23 @@
       <c r="K371" s="6" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="372" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L371" s="1">
+        <v>60</v>
+      </c>
+      <c r="M371" s="1">
+        <v>0</v>
+      </c>
+      <c r="N371" s="1">
+        <v>7</v>
+      </c>
+      <c r="O371" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="V371" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="372" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A372" s="3">
         <v>41789</v>
       </c>
@@ -14508,8 +15558,29 @@
       <c r="K372" s="6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L372" s="1">
+        <v>20</v>
+      </c>
+      <c r="M372" s="1">
+        <v>270</v>
+      </c>
+      <c r="N372" s="1">
+        <v>7</v>
+      </c>
+      <c r="O372" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q372" s="1">
+        <v>30</v>
+      </c>
+      <c r="T372" s="1">
+        <v>20</v>
+      </c>
+      <c r="V372" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="373" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A373" s="3">
         <v>41789</v>
       </c>
@@ -14543,8 +15614,26 @@
       <c r="K373" s="6" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L373" s="1">
+        <v>10</v>
+      </c>
+      <c r="M373" s="1">
+        <v>180</v>
+      </c>
+      <c r="N373" s="1">
+        <v>5</v>
+      </c>
+      <c r="O373" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R373" s="1">
+        <v>10</v>
+      </c>
+      <c r="T373" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="374" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A374" s="3">
         <v>41789</v>
       </c>
@@ -14579,7 +15668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="375" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A375" s="3">
         <v>41789</v>
       </c>
@@ -14613,8 +15702,26 @@
       <c r="K375" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L375" s="1">
+        <v>80</v>
+      </c>
+      <c r="M375" s="1">
+        <v>180</v>
+      </c>
+      <c r="N375" s="1">
+        <v>7</v>
+      </c>
+      <c r="O375" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S375" s="1">
+        <v>80</v>
+      </c>
+      <c r="V375" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="376" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A376" s="3">
         <v>41789</v>
       </c>
@@ -14649,7 +15756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A377" s="3">
         <v>41789</v>
       </c>
@@ -14684,7 +15791,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="378" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A378" s="3">
         <v>41789</v>
       </c>
@@ -14718,8 +15825,26 @@
       <c r="K378" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L378" s="1">
+        <v>50</v>
+      </c>
+      <c r="M378" s="1">
+        <v>90</v>
+      </c>
+      <c r="N378" s="1">
+        <v>4</v>
+      </c>
+      <c r="O378" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R378" s="1">
+        <v>50</v>
+      </c>
+      <c r="S378" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="379" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A379" s="3">
         <v>41789</v>
       </c>
@@ -14753,8 +15878,26 @@
       <c r="K379" s="6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="380" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L379" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M379" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N379" s="1">
+        <v>6</v>
+      </c>
+      <c r="O379" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q379" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U379" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="380" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A380" s="3">
         <v>41789</v>
       </c>
@@ -14788,8 +15931,26 @@
       <c r="K380" s="6" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="381" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L380" s="1">
+        <v>60</v>
+      </c>
+      <c r="M380" s="1">
+        <v>270</v>
+      </c>
+      <c r="N380" s="1">
+        <v>4</v>
+      </c>
+      <c r="O380" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R380" s="1">
+        <v>60</v>
+      </c>
+      <c r="S380" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="381" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A381" s="3">
         <v>41789</v>
       </c>
@@ -14823,8 +15984,26 @@
       <c r="K381" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="382" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L381" s="1">
+        <v>15</v>
+      </c>
+      <c r="M381" s="1">
+        <v>50</v>
+      </c>
+      <c r="N381" s="1">
+        <v>5</v>
+      </c>
+      <c r="O381" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R381" s="1">
+        <v>40</v>
+      </c>
+      <c r="T381" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="382" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A382" s="3">
         <v>41789</v>
       </c>
@@ -14858,8 +16037,26 @@
       <c r="K382" s="6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="383" spans="1:11" ht="61.2" x14ac:dyDescent="0.2">
+      <c r="L382" s="1">
+        <v>80</v>
+      </c>
+      <c r="M382" s="1">
+        <v>180</v>
+      </c>
+      <c r="N382" s="1">
+        <v>7</v>
+      </c>
+      <c r="O382" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S382" s="1">
+        <v>80</v>
+      </c>
+      <c r="V382" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="383" spans="1:22" ht="61.2" x14ac:dyDescent="0.2">
       <c r="A383" s="3">
         <v>41789</v>
       </c>
@@ -14893,8 +16090,26 @@
       <c r="K383" s="6" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L383" s="1">
+        <v>20</v>
+      </c>
+      <c r="M383" s="1">
+        <v>145</v>
+      </c>
+      <c r="N383" s="1">
+        <v>7</v>
+      </c>
+      <c r="O383" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="R383" s="1">
+        <v>30</v>
+      </c>
+      <c r="V383" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="384" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A384" s="3">
         <v>41789</v>
       </c>
@@ -14929,7 +16144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="385" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A385" s="8">
         <v>41817</v>
       </c>
@@ -14960,8 +16175,23 @@
       <c r="K385" s="6" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="386" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L385" s="1">
+        <v>25</v>
+      </c>
+      <c r="M385" s="1">
+        <v>345</v>
+      </c>
+      <c r="N385" s="1">
+        <v>2</v>
+      </c>
+      <c r="O385" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q385" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="386" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A386" s="8">
         <v>41817</v>
       </c>
@@ -14992,8 +16222,23 @@
       <c r="K386" s="6" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L386" s="1">
+        <v>70</v>
+      </c>
+      <c r="M386" s="1">
+        <v>180</v>
+      </c>
+      <c r="N386" s="1">
+        <v>2</v>
+      </c>
+      <c r="O386" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q386" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="387" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A387" s="8">
         <v>41817</v>
       </c>
@@ -15025,7 +16270,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="388" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A388" s="8">
         <v>41817</v>
       </c>
@@ -15056,8 +16301,23 @@
       <c r="K388" s="6" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L388" s="1">
+        <v>15</v>
+      </c>
+      <c r="M388" s="1">
+        <v>160</v>
+      </c>
+      <c r="N388" s="1">
+        <v>4</v>
+      </c>
+      <c r="O388" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S388" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="389" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A389" s="8">
         <v>41817</v>
       </c>
@@ -15088,8 +16348,23 @@
       <c r="K389" s="6" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="390" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+      <c r="L389" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M389" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N389" s="1">
+        <v>4</v>
+      </c>
+      <c r="O389" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S389" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="390" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A390" s="8">
         <v>41817</v>
       </c>
@@ -15120,8 +16395,32 @@
       <c r="K390" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L390" s="1">
+        <v>10</v>
+      </c>
+      <c r="M390" s="1">
+        <v>270</v>
+      </c>
+      <c r="N390" s="1">
+        <v>7</v>
+      </c>
+      <c r="O390" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q390" s="1">
+        <v>10</v>
+      </c>
+      <c r="S390" s="1">
+        <v>10</v>
+      </c>
+      <c r="U390" s="1">
+        <v>10</v>
+      </c>
+      <c r="V390" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="391" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A391" s="8">
         <v>41817</v>
       </c>
@@ -15153,7 +16452,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A392" s="8">
         <v>41817</v>
       </c>
@@ -15185,7 +16484,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="393" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A393" s="8">
         <v>41817</v>
       </c>
@@ -15216,8 +16515,29 @@
       <c r="K393" s="6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L393" s="1">
+        <v>10</v>
+      </c>
+      <c r="M393" s="1">
+        <v>160</v>
+      </c>
+      <c r="N393" s="1">
+        <v>6</v>
+      </c>
+      <c r="O393" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q393" s="1">
+        <v>10</v>
+      </c>
+      <c r="T393" s="1">
+        <v>10</v>
+      </c>
+      <c r="U393" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="394" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A394" s="8">
         <v>41817</v>
       </c>
@@ -15248,8 +16568,23 @@
       <c r="K394" s="6" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L394" s="1">
+        <v>40</v>
+      </c>
+      <c r="M394" s="1">
+        <v>90</v>
+      </c>
+      <c r="N394" s="1">
+        <v>2</v>
+      </c>
+      <c r="O394" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q394" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="395" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A395" s="8">
         <v>41817</v>
       </c>
@@ -15281,7 +16616,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="396" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A396" s="8">
         <v>41817</v>
       </c>
@@ -15312,8 +16647,26 @@
       <c r="K396" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L396" s="1">
+        <v>50</v>
+      </c>
+      <c r="M396" s="1">
+        <v>160</v>
+      </c>
+      <c r="N396" s="1">
+        <v>7</v>
+      </c>
+      <c r="O396" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="S396" s="1">
+        <v>80</v>
+      </c>
+      <c r="V396" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="397" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A397" s="8">
         <v>41817</v>
       </c>
@@ -15345,7 +16698,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A398" s="8">
         <v>41817</v>
       </c>
@@ -15377,7 +16730,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="399" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A399" s="8">
         <v>41817</v>
       </c>
@@ -15408,8 +16761,26 @@
       <c r="K399" s="7" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L399" s="1">
+        <v>15</v>
+      </c>
+      <c r="M399" s="1">
+        <v>180</v>
+      </c>
+      <c r="N399" s="1">
+        <v>6</v>
+      </c>
+      <c r="O399" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q399" s="1">
+        <v>30</v>
+      </c>
+      <c r="U399" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="400" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A400" s="8">
         <v>41817</v>
       </c>
@@ -15441,7 +16812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A401" s="8">
         <v>41817</v>
       </c>
@@ -15472,8 +16843,23 @@
       <c r="K401" s="6" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="402" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+      <c r="L401" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M401" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N401" s="1">
+        <v>2</v>
+      </c>
+      <c r="O401" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q401" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="402" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A402" s="8">
         <v>41817</v>
       </c>
@@ -15504,8 +16890,26 @@
       <c r="K402" s="6" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L402" s="1">
+        <v>5</v>
+      </c>
+      <c r="M402" s="1">
+        <v>100</v>
+      </c>
+      <c r="N402" s="1">
+        <v>6</v>
+      </c>
+      <c r="O402" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q402" s="1">
+        <v>10</v>
+      </c>
+      <c r="U402" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="403" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A403" s="8">
         <v>41817</v>
       </c>
@@ -15536,8 +16940,23 @@
       <c r="K403" s="6" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L403" s="1">
+        <v>30</v>
+      </c>
+      <c r="M403" s="1">
+        <v>25</v>
+      </c>
+      <c r="N403" s="1">
+        <v>2</v>
+      </c>
+      <c r="O403" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q403" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="404" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A404" s="8">
         <v>41817</v>
       </c>
@@ -15569,7 +16988,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A405" s="8">
         <v>41817</v>
       </c>
@@ -15601,7 +17020,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A406" s="8">
         <v>41817</v>
       </c>
@@ -15633,7 +17052,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="407" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A407" s="8">
         <v>41817</v>
       </c>
@@ -15664,8 +17083,20 @@
       <c r="K407" s="7" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L407" s="1">
+        <v>100</v>
+      </c>
+      <c r="M407" s="1">
+        <v>200</v>
+      </c>
+      <c r="N407" s="1">
+        <v>0</v>
+      </c>
+      <c r="O407" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="408" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A408" s="8">
         <v>41817</v>
       </c>
@@ -15696,8 +17127,23 @@
       <c r="K408" s="7" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L408" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M408" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N408" s="1">
+        <v>2</v>
+      </c>
+      <c r="O408" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q408" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="409" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A409" s="8">
         <v>41817</v>
       </c>
@@ -15728,8 +17174,23 @@
       <c r="K409" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="410" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L409" s="1">
+        <v>50</v>
+      </c>
+      <c r="M409" s="1">
+        <v>5</v>
+      </c>
+      <c r="N409" s="1">
+        <v>2</v>
+      </c>
+      <c r="O409" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q409" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="410" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A410" s="8">
         <v>41817</v>
       </c>
@@ -15760,8 +17221,20 @@
       <c r="K410" s="6" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L410" s="1">
+        <v>25</v>
+      </c>
+      <c r="M410" s="1">
+        <v>285</v>
+      </c>
+      <c r="N410" s="1">
+        <v>0</v>
+      </c>
+      <c r="O410" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="411" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A411" s="8">
         <v>41817</v>
       </c>
@@ -15793,7 +17266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="412" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A412" s="8">
         <v>41817</v>
       </c>
@@ -15824,8 +17297,32 @@
       <c r="K412" s="6" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L412" s="1">
+        <v>15</v>
+      </c>
+      <c r="M412" s="1">
+        <v>200</v>
+      </c>
+      <c r="N412" s="1">
+        <v>7</v>
+      </c>
+      <c r="O412" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q412" s="1">
+        <v>15</v>
+      </c>
+      <c r="T412" s="1">
+        <v>15</v>
+      </c>
+      <c r="U412" s="1">
+        <v>15</v>
+      </c>
+      <c r="V412" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="413" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A413" s="8">
         <v>41817</v>
       </c>
@@ -15857,7 +17354,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A414" s="8">
         <v>41817</v>
       </c>
@@ -15889,7 +17386,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="415" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:22" ht="51" x14ac:dyDescent="0.2">
       <c r="A415" s="8">
         <v>41817</v>
       </c>
@@ -15920,8 +17417,26 @@
       <c r="K415" s="7" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="416" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L415" s="1">
+        <v>5</v>
+      </c>
+      <c r="M415" s="1">
+        <v>180</v>
+      </c>
+      <c r="N415" s="1">
+        <v>5</v>
+      </c>
+      <c r="O415" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q415" s="1">
+        <v>10</v>
+      </c>
+      <c r="T415" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="416" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A416" s="8">
         <v>41817</v>
       </c>
@@ -15952,8 +17467,29 @@
       <c r="K416" s="7" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="417" spans="1:11" ht="40.799999999999997" x14ac:dyDescent="0.2">
+      <c r="L416" s="1">
+        <v>15</v>
+      </c>
+      <c r="M416" s="1">
+        <v>0</v>
+      </c>
+      <c r="N416" s="1">
+        <v>7</v>
+      </c>
+      <c r="O416" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q416" s="1">
+        <v>15</v>
+      </c>
+      <c r="U416" s="1">
+        <v>20</v>
+      </c>
+      <c r="V416" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="417" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
       <c r="A417" s="8">
         <v>41817</v>
       </c>
@@ -15984,8 +17520,29 @@
       <c r="K417" s="6" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="418" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L417" s="1">
+        <v>100</v>
+      </c>
+      <c r="M417" s="1">
+        <v>270</v>
+      </c>
+      <c r="N417" s="1">
+        <v>7</v>
+      </c>
+      <c r="O417" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R417" s="1">
+        <v>100</v>
+      </c>
+      <c r="S417" s="1">
+        <v>100</v>
+      </c>
+      <c r="V417" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="418" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A418" s="8">
         <v>41817</v>
       </c>
@@ -16016,8 +17573,26 @@
       <c r="K418" s="6" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="419" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="L418" s="1">
+        <v>10</v>
+      </c>
+      <c r="M418" s="1">
+        <v>355</v>
+      </c>
+      <c r="N418" s="1">
+        <v>7</v>
+      </c>
+      <c r="O418" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q418" s="1">
+        <v>10</v>
+      </c>
+      <c r="V418" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="419" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A419" s="8">
         <v>41817</v>
       </c>
@@ -16048,8 +17623,23 @@
       <c r="K419" s="6" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L419" s="1">
+        <v>15</v>
+      </c>
+      <c r="M419" s="1">
+        <v>270</v>
+      </c>
+      <c r="N419" s="1">
+        <v>2</v>
+      </c>
+      <c r="O419" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q419" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="420" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A420" s="8">
         <v>41817</v>
       </c>
@@ -16080,8 +17670,23 @@
       <c r="K420" s="6" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L420" s="1">
+        <v>70</v>
+      </c>
+      <c r="M420" s="1">
+        <v>90</v>
+      </c>
+      <c r="N420" s="1">
+        <v>3</v>
+      </c>
+      <c r="O420" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R420" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="421" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A421" s="8">
         <v>41817</v>
       </c>
@@ -16113,7 +17718,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A422" s="8">
         <v>41817</v>
       </c>
@@ -16145,7 +17750,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A423" s="8">
         <v>41817</v>
       </c>
@@ -16177,7 +17782,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A424" s="8">
         <v>41817</v>
       </c>
@@ -16209,7 +17814,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="425" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A425" s="8">
         <v>41817</v>
       </c>
@@ -16240,8 +17845,26 @@
       <c r="K425" s="6" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="426" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+      <c r="L425" s="1">
+        <v>15</v>
+      </c>
+      <c r="M425" s="1">
+        <v>270</v>
+      </c>
+      <c r="N425" s="1">
+        <v>6</v>
+      </c>
+      <c r="O425" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S425" s="1">
+        <v>15</v>
+      </c>
+      <c r="U425" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="426" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A426" s="8">
         <v>41817</v>
       </c>
@@ -16272,8 +17895,29 @@
       <c r="K426" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L426" s="1">
+        <v>10</v>
+      </c>
+      <c r="M426" s="1">
+        <v>270</v>
+      </c>
+      <c r="N426" s="1">
+        <v>7</v>
+      </c>
+      <c r="O426" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q426" s="1">
+        <v>10</v>
+      </c>
+      <c r="S426" s="1">
+        <v>15</v>
+      </c>
+      <c r="V426" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="427" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A427" s="8">
         <v>41817</v>
       </c>
@@ -16305,7 +17949,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A428" s="8">
         <v>41817</v>
       </c>
@@ -16337,7 +17981,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A429" s="8">
         <v>41817</v>
       </c>
@@ -16369,7 +18013,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A430" s="8">
         <v>41817</v>
       </c>
@@ -16401,7 +18045,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A431" s="8">
         <v>41817</v>
       </c>
@@ -16433,7 +18077,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A432" s="8">
         <v>41817</v>
       </c>
@@ -16463,6 +18107,18 @@
       </c>
       <c r="K432" s="7" t="s">
         <v>208</v>
+      </c>
+      <c r="L432" s="1">
+        <v>15</v>
+      </c>
+      <c r="M432" s="1">
+        <v>0</v>
+      </c>
+      <c r="N432" s="1">
+        <v>0</v>
+      </c>
+      <c r="O432" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.2">
@@ -16977,7 +18633,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A449" s="3">
         <v>41808</v>
       </c>
@@ -17009,7 +18665,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A450" s="3">
         <v>41808</v>
       </c>
@@ -17041,7 +18697,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A451" s="3">
         <v>41808</v>
       </c>
@@ -17073,7 +18729,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A452" s="3">
         <v>41808</v>
       </c>
@@ -17105,7 +18761,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A453" s="3">
         <v>41808</v>
       </c>
@@ -17137,7 +18793,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A454" s="3">
         <v>41808</v>
       </c>
@@ -17169,7 +18825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A455" s="3">
         <v>41808</v>
       </c>
@@ -17201,7 +18857,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A456" s="3">
         <v>41808</v>
       </c>
@@ -17232,8 +18888,26 @@
       <c r="K456" s="10" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L456" s="1">
+        <v>20</v>
+      </c>
+      <c r="M456" s="1">
+        <v>180</v>
+      </c>
+      <c r="N456" s="1">
+        <v>7</v>
+      </c>
+      <c r="O456" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q456" s="1">
+        <v>20</v>
+      </c>
+      <c r="V456" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="457" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A457" s="3">
         <v>41808</v>
       </c>
@@ -17265,7 +18939,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="458" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A458" s="3">
         <v>41808</v>
       </c>
@@ -17297,7 +18971,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="459" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A459" s="3">
         <v>41808</v>
       </c>
@@ -17328,8 +19002,23 @@
       <c r="K459" s="6" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="460" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L459" s="1">
+        <v>100</v>
+      </c>
+      <c r="M459" s="1">
+        <v>180</v>
+      </c>
+      <c r="N459" s="1">
+        <v>1</v>
+      </c>
+      <c r="O459" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="P459" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="460" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A460" s="3">
         <v>41808</v>
       </c>
@@ -17361,7 +19050,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="461" spans="1:11" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
       <c r="A461" s="3">
         <v>41808</v>
       </c>
@@ -17392,8 +19081,26 @@
       <c r="K461" s="6" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="462" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L461" s="1">
+        <v>30</v>
+      </c>
+      <c r="M461" s="1">
+        <v>0</v>
+      </c>
+      <c r="N461" s="1">
+        <v>6</v>
+      </c>
+      <c r="O461" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q461" s="1">
+        <v>30</v>
+      </c>
+      <c r="U461" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="462" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A462" s="3">
         <v>41808</v>
       </c>
@@ -17425,7 +19132,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="463" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A463" s="3">
         <v>41808</v>
       </c>
@@ -17457,7 +19164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="464" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A464" s="3">
         <v>41808</v>
       </c>
@@ -17489,7 +19196,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="465" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A465" s="3">
         <v>41808</v>
       </c>
@@ -17521,7 +19228,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="466" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A466" s="3">
         <v>41808</v>
       </c>
@@ -17553,7 +19260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="467" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A467" s="3">
         <v>41808</v>
       </c>
@@ -17585,7 +19292,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="468" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A468" s="3">
         <v>41808</v>
       </c>
@@ -17617,7 +19324,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="469" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A469" s="3">
         <v>41808</v>
       </c>
@@ -17649,7 +19356,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="470" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A470" s="3">
         <v>41808</v>
       </c>
@@ -17681,7 +19388,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="471" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A471" s="3">
         <v>41808</v>
       </c>
@@ -17713,7 +19420,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="472" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A472" s="3">
         <v>41808</v>
       </c>
@@ -17745,7 +19452,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="473" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A473" s="3">
         <v>41808</v>
       </c>
@@ -17777,7 +19484,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A474" s="3">
         <v>41808</v>
       </c>
@@ -17809,7 +19516,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="475" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A475" s="3">
         <v>41808</v>
       </c>
@@ -17840,8 +19547,23 @@
       <c r="K475" s="10" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L475" s="1">
+        <v>100</v>
+      </c>
+      <c r="M475" s="1">
+        <v>90</v>
+      </c>
+      <c r="N475" s="1">
+        <v>1</v>
+      </c>
+      <c r="O475" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="P475" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="476" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A476" s="3">
         <v>41808</v>
       </c>
@@ -17873,7 +19595,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A477" s="3">
         <v>41808</v>
       </c>
@@ -17905,7 +19627,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A478" s="3">
         <v>41808</v>
       </c>
@@ -17937,7 +19659,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A479" s="3">
         <v>41808</v>
       </c>
@@ -17969,7 +19691,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="480" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A480" s="3">
         <v>41808</v>
       </c>
@@ -18001,7 +19723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A481" s="3">
         <v>41808</v>
       </c>
@@ -18033,7 +19755,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="482" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A482" s="3">
         <v>41808</v>
       </c>
@@ -18065,7 +19787,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A483" s="3">
         <v>41808</v>
       </c>
@@ -18097,7 +19819,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="484" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A484" s="3">
         <v>41808</v>
       </c>
@@ -18127,6 +19849,21 @@
       </c>
       <c r="K484" s="10" t="s">
         <v>216</v>
+      </c>
+      <c r="L484" s="1">
+        <v>40</v>
+      </c>
+      <c r="M484" s="1">
+        <v>90</v>
+      </c>
+      <c r="N484" s="1">
+        <v>4</v>
+      </c>
+      <c r="O484" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="S484" s="1">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Values where no data given but bird was present coded as 9999 to distinguish from the blank cells (which will be NA) where bird did not exhibit a behavior.
</commit_message>
<xml_diff>
--- a/20170117_CASP_playback_responses_combined_longform.xlsx
+++ b/20170117_CASP_playback_responses_combined_longform.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2636" uniqueCount="231">
   <si>
     <t>Date</t>
   </si>
@@ -1139,10 +1139,10 @@
   <dimension ref="A1:V484"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="K450" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="I391" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L485" sqref="L485"/>
+      <selection pane="bottomRight" activeCell="Q408" sqref="P1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -1382,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -1446,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
@@ -1651,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -1683,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
@@ -1903,7 +1903,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
@@ -1935,7 +1935,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
@@ -1967,7 +1967,7 @@
         <v>0</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
@@ -1999,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
@@ -2081,7 +2081,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
@@ -2160,7 +2160,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
@@ -2224,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
@@ -2341,7 +2341,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
@@ -2373,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
@@ -2405,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.2">
@@ -2437,7 +2437,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.2">
@@ -2586,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.2">
@@ -2618,7 +2618,7 @@
         <v>0</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.2">
@@ -2650,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:22" x14ac:dyDescent="0.2">
@@ -2714,7 +2714,7 @@
         <v>0</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.2">
@@ -2746,7 +2746,7 @@
         <v>0</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:22" x14ac:dyDescent="0.2">
@@ -2778,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.2">
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45" spans="1:22" x14ac:dyDescent="0.2">
@@ -2842,7 +2842,7 @@
         <v>0</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.2">
@@ -2874,7 +2874,7 @@
         <v>0</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.2">
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.2">
@@ -2938,7 +2938,7 @@
         <v>0</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.2">
@@ -3017,7 +3017,7 @@
         <v>0</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.2">
@@ -3049,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.2">
@@ -3081,7 +3081,7 @@
         <v>0</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.2">
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.2">
@@ -3239,7 +3239,7 @@
         <v>0</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.2">
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:22" x14ac:dyDescent="0.2">
@@ -3309,7 +3309,7 @@
         <v>0</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.2">
@@ -3344,7 +3344,7 @@
         <v>0</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.2">
@@ -3432,7 +3432,7 @@
         <v>0</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:22" x14ac:dyDescent="0.2">
@@ -3467,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.2">
@@ -3502,7 +3502,7 @@
         <v>0</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:22" x14ac:dyDescent="0.2">
@@ -3590,7 +3590,7 @@
         <v>0</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
@@ -3625,7 +3625,7 @@
         <v>0</v>
       </c>
       <c r="K66" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
@@ -3660,7 +3660,7 @@
         <v>0</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
@@ -3695,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="K68" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
@@ -3730,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.2">
@@ -3765,7 +3765,7 @@
         <v>0</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
@@ -3800,7 +3800,7 @@
         <v>0</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -3870,7 +3870,7 @@
         <v>0</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:20" ht="30.6" x14ac:dyDescent="0.2">
@@ -3958,7 +3958,7 @@
         <v>0</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
@@ -4043,7 +4043,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
@@ -4078,7 +4078,7 @@
         <v>0</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:20" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5077,8 +5077,8 @@
       <c r="O101" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="V101" s="1" t="s">
-        <v>22</v>
+      <c r="V101" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="102" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5118,11 +5118,11 @@
       <c r="O102" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="Q102" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V102" s="1" t="s">
-        <v>22</v>
+      <c r="Q102" s="1">
+        <v>9999</v>
+      </c>
+      <c r="V102" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.2">
@@ -5482,8 +5482,8 @@
       <c r="O110" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="V110" s="1" t="s">
-        <v>22</v>
+      <c r="V110" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="111" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -6525,8 +6525,8 @@
       <c r="O138" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="R138" s="1" t="s">
-        <v>22</v>
+      <c r="R138" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="139" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
@@ -6572,11 +6572,11 @@
       <c r="O139" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="R139" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T139" s="1" t="s">
-        <v>22</v>
+      <c r="R139" s="1">
+        <v>9999</v>
+      </c>
+      <c r="T139" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="140" spans="1:22" x14ac:dyDescent="0.2">
@@ -12513,8 +12513,8 @@
       <c r="O297" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="U297" s="1" t="s">
-        <v>22</v>
+      <c r="U297" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="298" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -12759,8 +12759,8 @@
       <c r="O303" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Q303" s="1" t="s">
-        <v>22</v>
+      <c r="Q303" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="304" spans="1:22" x14ac:dyDescent="0.2">
@@ -12891,8 +12891,8 @@
       <c r="O306" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="V306" s="1" t="s">
-        <v>22</v>
+      <c r="V306" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="307" spans="1:22" x14ac:dyDescent="0.2">
@@ -13201,8 +13201,8 @@
       <c r="O314" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="R314" s="1" t="s">
-        <v>22</v>
+      <c r="R314" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="315" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -13912,11 +13912,11 @@
       <c r="O332" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Q332" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V332" s="1" t="s">
-        <v>22</v>
+      <c r="Q332" s="1">
+        <v>9999</v>
+      </c>
+      <c r="V332" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="333" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -14272,8 +14272,8 @@
       <c r="O341" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Q341" s="1" t="s">
-        <v>22</v>
+      <c r="Q341" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="342" spans="1:22" x14ac:dyDescent="0.2">
@@ -15400,8 +15400,8 @@
       <c r="O368" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="P368" s="1" t="s">
-        <v>22</v>
+      <c r="P368" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="369" spans="1:22" x14ac:dyDescent="0.2">
@@ -15890,11 +15890,11 @@
       <c r="O379" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Q379" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="U379" s="1" t="s">
-        <v>22</v>
+      <c r="Q379" s="1">
+        <v>9999</v>
+      </c>
+      <c r="U379" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="380" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -16360,8 +16360,8 @@
       <c r="O389" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="S389" s="1" t="s">
-        <v>22</v>
+      <c r="S389" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="390" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
@@ -16855,8 +16855,8 @@
       <c r="O401" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="Q401" s="1" t="s">
-        <v>22</v>
+      <c r="Q401" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="402" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
@@ -17139,8 +17139,8 @@
       <c r="O408" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="Q408" s="1" t="s">
-        <v>22</v>
+      <c r="Q408" s="1">
+        <v>9999</v>
       </c>
     </row>
     <row r="409" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>